<commit_message>
Adding method 'Model.check_model_results()' to compare data of model with expected data. Methods called in the tests. Now working on fixing all test models.
</commit_message>
<xml_diff>
--- a/tests/integration/units/constants/input_data/input_data.xlsx
+++ b/tests/integration/units/constants/input_data/input_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\fixtures\constants\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\integration\units\constants\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8FDCB7-4A8F-482C-986F-148A9EEFE563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D79C605-99B3-42BD-8490-36087F17FFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32180" yWindow="2500" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Q" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>c_Name</t>
-  </si>
-  <si>
     <t>f_Name</t>
   </si>
   <si>
     <t>values</t>
-  </si>
-  <si>
-    <t>base</t>
   </si>
   <si>
     <t>oil products</t>
@@ -412,18 +406,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="3" width="17.26953125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,77 +424,59 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
+      <c r="C3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="C4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="C6">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Github issue #62 solved: improving Model.Core.data_tocvxpy_exogenous_vars() method by checking allowed values type in source data before assign them to variables. Allowed types for values defined in Constants.
</commit_message>
<xml_diff>
--- a/tests/integration/units/constants/input_data/input_data.xlsx
+++ b/tests/integration/units/constants/input_data/input_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\integration\units\constants\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D79C605-99B3-42BD-8490-36087F17FFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FD1A64-4DA1-4EB5-A9D6-BB665C9A3FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -409,7 +409,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Modifying 'constant' unit problem. Adding tests to test_util.py module.
</commit_message>
<xml_diff>
--- a/tests/integration/units/constants/input_data/input_data.xlsx
+++ b/tests/integration/units/constants/input_data/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\integration\units\constants\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FD1A64-4DA1-4EB5-A9D6-BB665C9A3FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F0ECF4-904B-4435-A2CD-B4F76B9894F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24850" yWindow="3390" windowWidth="16140" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Q" sheetId="1" r:id="rId1"/>

</xml_diff>